<commit_message>
created excel of betas
</commit_message>
<xml_diff>
--- a/Participant_Betas.xlsx
+++ b/Participant_Betas.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Betas</t>
+  </si>
   <si>
     <t>00001</t>
   </si>
@@ -464,262 +470,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1">
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2">
+        <v>74</v>
+      </c>
+      <c r="C2">
         <v>0.1040163724753834</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="C3">
         <v>0.1131581030593162</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
+        <v>67</v>
+      </c>
+      <c r="C4">
         <v>-0.704839171694376</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
+        <v>70</v>
+      </c>
+      <c r="C5">
         <v>-0.1042528061966274</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6">
+        <v>80</v>
+      </c>
+      <c r="C6">
         <v>0.1874588139181941</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
+        <v>70</v>
+      </c>
+      <c r="C7">
         <v>-0.106336945396442</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8">
+        <v>67</v>
+      </c>
+      <c r="C8">
         <v>0.3304904913413018</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9">
+        <v>73</v>
+      </c>
+      <c r="C9">
         <v>0.4219051765703421</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10">
+        <v>74</v>
+      </c>
+      <c r="C10">
         <v>0.3994876068207415</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11">
+        <v>72</v>
+      </c>
+      <c r="C11">
         <v>0.223170839991305</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12">
+        <v>76</v>
+      </c>
+      <c r="C12">
         <v>0.150948677317973</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13">
+        <v>71</v>
+      </c>
+      <c r="C13">
         <v>-0.3500238771328504</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14">
+        <v>70</v>
+      </c>
+      <c r="C14">
         <v>-0.09444878724401627</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15">
+        <v>69</v>
+      </c>
+      <c r="C15">
         <v>0.5624575368434465</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16">
+        <v>68</v>
+      </c>
+      <c r="C16">
         <v>0.2344792956722706</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17">
+        <v>73</v>
+      </c>
+      <c r="C17">
         <v>-0.06973977912573877</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18">
+        <v>73</v>
+      </c>
+      <c r="C18">
         <v>0.8518252964915777</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19">
+        <v>70</v>
+      </c>
+      <c r="C19">
         <v>-0.1454541336370711</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20">
+        <v>66</v>
+      </c>
+      <c r="C20">
         <v>-0.4106516063996151</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B21">
+        <v>67</v>
+      </c>
+      <c r="C21">
         <v>-0.2041764779054052</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B22">
+        <v>86</v>
+      </c>
+      <c r="C22">
         <v>-0.6473642535309051</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B23">
+        <v>73</v>
+      </c>
+      <c r="C23">
         <v>-0.591904249299756</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B24">
+        <v>66</v>
+      </c>
+      <c r="C24">
         <v>-0.4124219974381256</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B25">
+        <v>69</v>
+      </c>
+      <c r="C25">
         <v>0.2179347960983495</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B26">
+        <v>75</v>
+      </c>
+      <c r="C26">
         <v>-0.120381292784837</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B27">
+        <v>72</v>
+      </c>
+      <c r="C27">
         <v>-0.1083154279602604</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28">
+        <v>75</v>
+      </c>
+      <c r="C28">
         <v>0.2435844343692198</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B29">
+        <v>71</v>
+      </c>
+      <c r="C29">
         <v>0.346014512136379</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B30">
+        <v>61</v>
+      </c>
+      <c r="C30">
         <v>-0.1559637165049998</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B31">
+        <v>69</v>
+      </c>
+      <c r="C31">
         <v>0.2240929776084732</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32">
+        <v>70</v>
+      </c>
+      <c r="C32">
         <v>-0.3759926832486572</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed betas and updated graphing
</commit_message>
<xml_diff>
--- a/Participant_Betas.xlsx
+++ b/Participant_Betas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Age</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>00104</t>
-  </si>
-  <si>
-    <t>00106</t>
   </si>
   <si>
     <t>00108</t>
@@ -470,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,7 +489,7 @@
         <v>74</v>
       </c>
       <c r="C2">
-        <v>0.1040163724753834</v>
+        <v>-0.08195218164326586</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -503,7 +500,7 @@
         <v>75</v>
       </c>
       <c r="C3">
-        <v>0.1131581030593162</v>
+        <v>0.6568106501272286</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -514,7 +511,7 @@
         <v>67</v>
       </c>
       <c r="C4">
-        <v>-0.704839171694376</v>
+        <v>0.6174199209563125</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -525,7 +522,7 @@
         <v>70</v>
       </c>
       <c r="C5">
-        <v>-0.1042528061966274</v>
+        <v>0.8433420439841035</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -536,7 +533,7 @@
         <v>80</v>
       </c>
       <c r="C6">
-        <v>0.1874588139181941</v>
+        <v>0.9207427672563853</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -547,7 +544,7 @@
         <v>70</v>
       </c>
       <c r="C7">
-        <v>-0.106336945396442</v>
+        <v>-0.8369058374174531</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -558,7 +555,7 @@
         <v>67</v>
       </c>
       <c r="C8">
-        <v>0.3304904913413018</v>
+        <v>-0.146261406513147</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -569,7 +566,7 @@
         <v>73</v>
       </c>
       <c r="C9">
-        <v>0.4219051765703421</v>
+        <v>-0.2610440497511629</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -580,7 +577,7 @@
         <v>74</v>
       </c>
       <c r="C10">
-        <v>0.3994876068207415</v>
+        <v>0.3219532911962275</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -591,7 +588,7 @@
         <v>72</v>
       </c>
       <c r="C11">
-        <v>0.223170839991305</v>
+        <v>0.5212777718618362</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -602,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="C12">
-        <v>0.150948677317973</v>
+        <v>0.7335304552149003</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -613,7 +610,7 @@
         <v>71</v>
       </c>
       <c r="C13">
-        <v>-0.3500238771328504</v>
+        <v>0.2892261725922131</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -624,7 +621,7 @@
         <v>70</v>
       </c>
       <c r="C14">
-        <v>-0.09444878724401627</v>
+        <v>0.771331611687378</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -635,7 +632,7 @@
         <v>69</v>
       </c>
       <c r="C15">
-        <v>0.5624575368434465</v>
+        <v>0.1334225975328344</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -646,7 +643,7 @@
         <v>68</v>
       </c>
       <c r="C16">
-        <v>0.2344792956722706</v>
+        <v>2.050372167566059</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -657,7 +654,7 @@
         <v>73</v>
       </c>
       <c r="C17">
-        <v>-0.06973977912573877</v>
+        <v>0.1795704815443444</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -668,7 +665,7 @@
         <v>73</v>
       </c>
       <c r="C18">
-        <v>0.8518252964915777</v>
+        <v>0.8103745525130024</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -679,7 +676,7 @@
         <v>70</v>
       </c>
       <c r="C19">
-        <v>-0.1454541336370711</v>
+        <v>0.6182454285682549</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -690,7 +687,7 @@
         <v>66</v>
       </c>
       <c r="C20">
-        <v>-0.4106516063996151</v>
+        <v>0.9386529878247606</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -701,7 +698,7 @@
         <v>67</v>
       </c>
       <c r="C21">
-        <v>-0.2041764779054052</v>
+        <v>0.3187844895085998</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -712,7 +709,7 @@
         <v>86</v>
       </c>
       <c r="C22">
-        <v>-0.6473642535309051</v>
+        <v>0.7374836884205355</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -720,10 +717,10 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C23">
-        <v>-0.591904249299756</v>
+        <v>0.3802788640284571</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -731,10 +728,10 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C24">
-        <v>-0.4124219974381256</v>
+        <v>1.104858743745738</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -742,10 +739,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C25">
-        <v>0.2179347960983495</v>
+        <v>1.315290685482777</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -753,10 +750,10 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C26">
-        <v>-0.120381292784837</v>
+        <v>0.6977254268521721</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -764,10 +761,10 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C27">
-        <v>-0.1083154279602604</v>
+        <v>1.044920483293541</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -775,10 +772,10 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C28">
-        <v>0.2435844343692198</v>
+        <v>0.6423057088524229</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -786,10 +783,10 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C29">
-        <v>0.346014512136379</v>
+        <v>0.9471158104941518</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -797,10 +794,10 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C30">
-        <v>-0.1559637165049998</v>
+        <v>0.8354543934670168</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -808,21 +805,10 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C31">
-        <v>0.2240929776084732</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32">
-        <v>70</v>
-      </c>
-      <c r="C32">
-        <v>-0.3759926832486572</v>
+        <v>0.4839018293907714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added p-values and updated graphing
</commit_message>
<xml_diff>
--- a/Participant_Betas.xlsx
+++ b/Participant_Betas.xlsx
@@ -489,7 +489,7 @@
         <v>74</v>
       </c>
       <c r="C2">
-        <v>-0.08195218164326586</v>
+        <v>0.0165316589608312</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -500,7 +500,7 @@
         <v>75</v>
       </c>
       <c r="C3">
-        <v>0.6568106501272286</v>
+        <v>0.1596747772390028</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -511,7 +511,7 @@
         <v>67</v>
       </c>
       <c r="C4">
-        <v>0.6174199209563125</v>
+        <v>0.8924876052044113</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -522,7 +522,7 @@
         <v>70</v>
       </c>
       <c r="C5">
-        <v>0.8433420439841035</v>
+        <v>0.7209875032280612</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -533,7 +533,7 @@
         <v>80</v>
       </c>
       <c r="C6">
-        <v>0.9207427672563853</v>
+        <v>0.9952126454880028</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -544,7 +544,7 @@
         <v>70</v>
       </c>
       <c r="C7">
-        <v>-0.8369058374174531</v>
+        <v>-0.001024306990703626</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -555,7 +555,7 @@
         <v>67</v>
       </c>
       <c r="C8">
-        <v>-0.146261406513147</v>
+        <v>-0.09342248582433159</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -566,7 +566,7 @@
         <v>73</v>
       </c>
       <c r="C9">
-        <v>-0.2610440497511629</v>
+        <v>-0.2773457422942077</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -577,7 +577,7 @@
         <v>74</v>
       </c>
       <c r="C10">
-        <v>0.3219532911962275</v>
+        <v>0.673185173740518</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -588,7 +588,7 @@
         <v>72</v>
       </c>
       <c r="C11">
-        <v>0.5212777718618362</v>
+        <v>-0.8972713613521036</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -599,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="C12">
-        <v>0.7335304552149003</v>
+        <v>0.7655094493981847</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -610,7 +610,7 @@
         <v>71</v>
       </c>
       <c r="C13">
-        <v>0.2892261725922131</v>
+        <v>0.1599476620886939</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -621,7 +621,7 @@
         <v>70</v>
       </c>
       <c r="C14">
-        <v>0.771331611687378</v>
+        <v>0.3444026411998959</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -632,7 +632,7 @@
         <v>69</v>
       </c>
       <c r="C15">
-        <v>0.1334225975328344</v>
+        <v>0.07589299699726311</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -643,7 +643,7 @@
         <v>68</v>
       </c>
       <c r="C16">
-        <v>2.050372167566059</v>
+        <v>2.453088300160251</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -654,7 +654,7 @@
         <v>73</v>
       </c>
       <c r="C17">
-        <v>0.1795704815443444</v>
+        <v>-0.1549791377016192</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -665,7 +665,7 @@
         <v>73</v>
       </c>
       <c r="C18">
-        <v>0.8103745525130024</v>
+        <v>0.7546548098942604</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -676,7 +676,7 @@
         <v>70</v>
       </c>
       <c r="C19">
-        <v>0.6182454285682549</v>
+        <v>0.2903360318096634</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -687,7 +687,7 @@
         <v>66</v>
       </c>
       <c r="C20">
-        <v>0.9386529878247606</v>
+        <v>0.6557382247212946</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -698,7 +698,7 @@
         <v>67</v>
       </c>
       <c r="C21">
-        <v>0.3187844895085998</v>
+        <v>0.8294043729654725</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -709,7 +709,7 @@
         <v>86</v>
       </c>
       <c r="C22">
-        <v>0.7374836884205355</v>
+        <v>0.7192499639843549</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -720,7 +720,7 @@
         <v>66</v>
       </c>
       <c r="C23">
-        <v>0.3802788640284571</v>
+        <v>0.4887190027762116</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -731,7 +731,7 @@
         <v>69</v>
       </c>
       <c r="C24">
-        <v>1.104858743745738</v>
+        <v>1.715815238194143</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -742,7 +742,7 @@
         <v>75</v>
       </c>
       <c r="C25">
-        <v>1.315290685482777</v>
+        <v>1.264219810813607</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -753,7 +753,7 @@
         <v>72</v>
       </c>
       <c r="C26">
-        <v>0.6977254268521721</v>
+        <v>0.9808549446337534</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -764,7 +764,7 @@
         <v>75</v>
       </c>
       <c r="C27">
-        <v>1.044920483293541</v>
+        <v>0.3866366398948996</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -775,7 +775,7 @@
         <v>71</v>
       </c>
       <c r="C28">
-        <v>0.6423057088524229</v>
+        <v>0.4914602873909288</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -786,7 +786,7 @@
         <v>61</v>
       </c>
       <c r="C29">
-        <v>0.9471158104941518</v>
+        <v>0.8003563227094359</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -797,7 +797,7 @@
         <v>69</v>
       </c>
       <c r="C30">
-        <v>0.8354543934670168</v>
+        <v>0.7361494804832538</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -808,7 +808,7 @@
         <v>70</v>
       </c>
       <c r="C31">
-        <v>0.4839018293907714</v>
+        <v>0.7587805559099209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
displaying two betas instead of one
</commit_message>
<xml_diff>
--- a/Participant_Betas.xlsx
+++ b/Participant_Betas.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>Age</t>
   </si>
   <si>
-    <t>Betas</t>
+    <t>MB_Betas</t>
+  </si>
+  <si>
+    <t>MF_Betas</t>
   </si>
   <si>
     <t>00001</t>
@@ -116,26 +119,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -150,35 +149,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -466,352 +456,451 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
         <v>74</v>
       </c>
-      <c r="C2">
-        <v>0.0165316589608312</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" t="n">
+        <v>0.01653165896082897</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.5379881714975817</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
         <v>75</v>
       </c>
-      <c r="C3">
-        <v>0.1596747772390028</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" t="n">
+        <v>0.1596747772390038</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.089894039326496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
         <v>67</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>0.8924876052044113</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="n">
+        <v>1.391851840185988</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
         <v>70</v>
       </c>
-      <c r="C5">
-        <v>0.7209875032280612</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" t="n">
+        <v>0.7209875032280563</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.503805907951867</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="n">
         <v>80</v>
       </c>
-      <c r="C6">
-        <v>0.9952126454880028</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" t="n">
+        <v>0.995212645488007</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.768571715121633</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="n">
         <v>70</v>
       </c>
-      <c r="C7">
-        <v>-0.001024306990703626</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" t="n">
+        <v>-0.001024306990703917</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.7320766699843498</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="n">
         <v>67</v>
       </c>
-      <c r="C8">
-        <v>-0.09342248582433159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" t="n">
+        <v>-0.09342248582433064</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.468304716247627</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="n">
         <v>73</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>-0.2773457422942077</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="n">
+        <v>0.8124973825454734</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="n">
         <v>74</v>
       </c>
-      <c r="C10">
-        <v>0.673185173740518</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10" t="n">
+        <v>0.6731851737405319</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.2902958805659071</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="B11" t="n">
         <v>72</v>
       </c>
-      <c r="C11">
-        <v>-0.8972713613521036</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11" t="n">
+        <v>-0.8972713613520993</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.6666276126663441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
+        <v>13</v>
+      </c>
+      <c r="B12" t="n">
         <v>76</v>
       </c>
-      <c r="C12">
-        <v>0.7655094493981847</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12" t="n">
+        <v>0.7655094493981848</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2.203408941684844</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="n">
         <v>71</v>
       </c>
-      <c r="C13">
-        <v>0.1599476620886939</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="C13" t="n">
+        <v>0.1599476620886868</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.4965622015633681</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="n">
         <v>70</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>0.3444026411998959</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="n">
+        <v>1.150461883737294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="B15" t="n">
         <v>69</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>0.07589299699726311</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="n">
+        <v>0.6132613389843293</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
+        <v>17</v>
+      </c>
+      <c r="B16" t="n">
         <v>68</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>2.453088300160251</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="n">
+        <v>0.1883035617989823</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
+        <v>18</v>
+      </c>
+      <c r="B17" t="n">
         <v>73</v>
       </c>
-      <c r="C17">
-        <v>-0.1549791377016192</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="C17" t="n">
+        <v>-0.1549791377016193</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.031807931177911</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
+        <v>19</v>
+      </c>
+      <c r="B18" t="n">
         <v>73</v>
       </c>
-      <c r="C18">
-        <v>0.7546548098942604</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="C18" t="n">
+        <v>0.7546548098942556</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.320005019777746</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="B19" t="n">
         <v>70</v>
       </c>
-      <c r="C19">
-        <v>0.2903360318096634</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="C19" t="n">
+        <v>0.2903360318096648</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.633384050140805</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
+        <v>21</v>
+      </c>
+      <c r="B20" t="n">
         <v>66</v>
       </c>
-      <c r="C20">
-        <v>0.6557382247212946</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="C20" t="n">
+        <v>0.6557382247212916</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.8038063877733496</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21">
+        <v>22</v>
+      </c>
+      <c r="B21" t="n">
         <v>67</v>
       </c>
-      <c r="C21">
-        <v>0.8294043729654725</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="C21" t="n">
+        <v>0.8294043729654733</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.4267165768561051</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
+        <v>23</v>
+      </c>
+      <c r="B22" t="n">
         <v>86</v>
       </c>
-      <c r="C22">
-        <v>0.7192499639843549</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="C22" t="n">
+        <v>0.7192499639843546</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.683853624525744</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23">
+        <v>24</v>
+      </c>
+      <c r="B23" t="n">
         <v>66</v>
       </c>
-      <c r="C23">
-        <v>0.4887190027762116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="C23" t="n">
+        <v>0.4887190027762117</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.140674008803199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
+        <v>25</v>
+      </c>
+      <c r="B24" t="n">
         <v>69</v>
       </c>
-      <c r="C24">
-        <v>1.715815238194143</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="C24" t="n">
+        <v>1.715815238194145</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.602353515373593</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25">
+        <v>26</v>
+      </c>
+      <c r="B25" t="n">
         <v>75</v>
       </c>
-      <c r="C25">
-        <v>1.264219810813607</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="C25" t="n">
+        <v>1.264219810813608</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2.485333829057352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26">
+        <v>27</v>
+      </c>
+      <c r="B26" t="n">
         <v>72</v>
       </c>
-      <c r="C26">
-        <v>0.9808549446337534</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="C26" t="n">
+        <v>0.9808549446337536</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.930322094548117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
+        <v>28</v>
+      </c>
+      <c r="B27" t="n">
         <v>75</v>
       </c>
-      <c r="C27">
-        <v>0.3866366398948996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="C27" t="n">
+        <v>0.3866366398948997</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.413531659103394</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28">
+        <v>29</v>
+      </c>
+      <c r="B28" t="n">
         <v>71</v>
       </c>
-      <c r="C28">
-        <v>0.4914602873909288</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="C28" t="n">
+        <v>0.4914602873909301</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.62819300270981</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29">
+        <v>30</v>
+      </c>
+      <c r="B29" t="n">
         <v>61</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="n">
         <v>0.8003563227094359</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" t="n">
+        <v>0.5148854143711534</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="n">
         <v>69</v>
       </c>
-      <c r="C30">
-        <v>0.7361494804832538</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="C30" t="n">
+        <v>0.7361494804832518</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.9022628061606567</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31">
+        <v>32</v>
+      </c>
+      <c r="B31" t="n">
         <v>70</v>
       </c>
-      <c r="C31">
-        <v>0.7587805559099209</v>
+      <c r="C31" t="n">
+        <v>0.7587805559099208</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.629361355435436</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel has all betas
</commit_message>
<xml_diff>
--- a/Participant_Betas.xlsx
+++ b/Participant_Betas.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Age</t>
   </si>
   <si>
-    <t>MB_Betas</t>
-  </si>
-  <si>
-    <t>MF_Betas</t>
+    <t>TT_Betas</t>
+  </si>
+  <si>
+    <t>R_Betas</t>
+  </si>
+  <si>
+    <t>Inter_Betas</t>
   </si>
   <si>
     <t>00001</t>
@@ -119,22 +122,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -149,26 +156,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -456,20 +472,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,428 +489,521 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>74</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.01653165896082897</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2">
+        <v>-0.0809690839194608</v>
+      </c>
+      <c r="D2">
         <v>0.5379881714975817</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>0.0165316589608312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3">
         <v>75</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.1596747772390038</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2.089894039326496</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="C3">
+        <v>0.05295669150259745</v>
+      </c>
+      <c r="D3">
+        <v>2.089894039326498</v>
+      </c>
+      <c r="E3">
+        <v>0.1596747772390028</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B4">
         <v>67</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
+        <v>0.05302163413420923</v>
+      </c>
+      <c r="D4">
+        <v>1.391851840185988</v>
+      </c>
+      <c r="E4">
         <v>0.8924876052044113</v>
       </c>
-      <c r="D4" t="n">
-        <v>1.391851840185988</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5">
         <v>70</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.7209875032280563</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2.503805907951867</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="C5">
+        <v>-0.09906011907041658</v>
+      </c>
+      <c r="D5">
+        <v>2.503805907951865</v>
+      </c>
+      <c r="E5">
+        <v>0.7209875032280612</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6">
         <v>80</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.995212645488007</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2.768571715121633</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="C6">
+        <v>0.001860099734153889</v>
+      </c>
+      <c r="D6">
+        <v>2.768571715121638</v>
+      </c>
+      <c r="E6">
+        <v>0.9952126454880028</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B7">
         <v>70</v>
       </c>
-      <c r="C7" t="n">
-        <v>-0.001024306990703917</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.7320766699843498</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="C7">
+        <v>-0.2273836202319065</v>
+      </c>
+      <c r="D7">
+        <v>0.7320766699843505</v>
+      </c>
+      <c r="E7">
+        <v>-0.001024306990703626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="n">
+        <v>10</v>
+      </c>
+      <c r="B8">
         <v>67</v>
       </c>
-      <c r="C8" t="n">
-        <v>-0.09342248582433064</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2.468304716247627</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="C8">
+        <v>0.4129843543178799</v>
+      </c>
+      <c r="D8">
+        <v>2.468304716247624</v>
+      </c>
+      <c r="E8">
+        <v>-0.09342248582433159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9">
         <v>73</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
+        <v>0.2929252863904141</v>
+      </c>
+      <c r="D9">
+        <v>0.8124973825454735</v>
+      </c>
+      <c r="E9">
         <v>-0.2773457422942077</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.8124973825454734</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="n">
+        <v>12</v>
+      </c>
+      <c r="B10">
         <v>74</v>
       </c>
-      <c r="C10" t="n">
-        <v>0.6731851737405319</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-0.2902958805659071</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="C10">
+        <v>-0.4794790883939876</v>
+      </c>
+      <c r="D10">
+        <v>-0.2902958805658937</v>
+      </c>
+      <c r="E10">
+        <v>0.673185173740518</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="n">
+        <v>13</v>
+      </c>
+      <c r="B11">
         <v>72</v>
       </c>
-      <c r="C11" t="n">
-        <v>-0.8972713613520993</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.6666276126663441</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="C11">
+        <v>-0.1171474774974689</v>
+      </c>
+      <c r="D11">
+        <v>0.6666276126663399</v>
+      </c>
+      <c r="E11">
+        <v>-0.8972713613521036</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12">
         <v>76</v>
       </c>
-      <c r="C12" t="n">
-        <v>0.7655094493981848</v>
-      </c>
-      <c r="D12" t="n">
+      <c r="C12">
+        <v>-0.3510635339666844</v>
+      </c>
+      <c r="D12">
         <v>2.203408941684844</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>0.7655094493981847</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="n">
+        <v>15</v>
+      </c>
+      <c r="B13">
         <v>71</v>
       </c>
-      <c r="C13" t="n">
-        <v>0.1599476620886868</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-0.4965622015633681</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="C13">
+        <v>-0.1340342982792192</v>
+      </c>
+      <c r="D13">
+        <v>-0.4965622015633767</v>
+      </c>
+      <c r="E13">
+        <v>0.1599476620886939</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="n">
+        <v>16</v>
+      </c>
+      <c r="B14">
         <v>70</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
+        <v>-0.3271492375885275</v>
+      </c>
+      <c r="D14">
+        <v>1.150461883737294</v>
+      </c>
+      <c r="E14">
         <v>0.3444026411998959</v>
       </c>
-      <c r="D14" t="n">
-        <v>1.150461883737294</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="n">
+        <v>17</v>
+      </c>
+      <c r="B15">
         <v>69</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
+        <v>0.4913704967036833</v>
+      </c>
+      <c r="D15">
+        <v>0.6132613389843292</v>
+      </c>
+      <c r="E15">
         <v>0.07589299699726311</v>
       </c>
-      <c r="D15" t="n">
-        <v>0.6132613389843293</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="n">
+        <v>18</v>
+      </c>
+      <c r="B16">
         <v>68</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
+        <v>0.2570356124660077</v>
+      </c>
+      <c r="D16">
+        <v>0.1883035617989822</v>
+      </c>
+      <c r="E16">
         <v>2.453088300160251</v>
       </c>
-      <c r="D16" t="n">
-        <v>0.1883035617989823</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="n">
+        <v>19</v>
+      </c>
+      <c r="B17">
         <v>73</v>
       </c>
-      <c r="C17" t="n">
-        <v>-0.1549791377016193</v>
-      </c>
-      <c r="D17" t="n">
+      <c r="C17">
+        <v>-0.2980432506103301</v>
+      </c>
+      <c r="D17">
         <v>1.031807931177911</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>-0.1549791377016192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="n">
+        <v>20</v>
+      </c>
+      <c r="B18">
         <v>73</v>
       </c>
-      <c r="C18" t="n">
-        <v>0.7546548098942556</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1.320005019777746</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="C18">
+        <v>-0.323449406699225</v>
+      </c>
+      <c r="D18">
+        <v>1.320005019777744</v>
+      </c>
+      <c r="E18">
+        <v>0.7546548098942604</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="n">
+        <v>21</v>
+      </c>
+      <c r="B19">
         <v>70</v>
       </c>
-      <c r="C19" t="n">
-        <v>0.2903360318096648</v>
-      </c>
-      <c r="D19" t="n">
-        <v>2.633384050140805</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="C19">
+        <v>-0.124573762622445</v>
+      </c>
+      <c r="D19">
+        <v>2.633384050140807</v>
+      </c>
+      <c r="E19">
+        <v>0.2903360318096634</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="n">
+        <v>22</v>
+      </c>
+      <c r="B20">
         <v>66</v>
       </c>
-      <c r="C20" t="n">
-        <v>0.6557382247212916</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.8038063877733496</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="C20">
+        <v>-0.7566753417719838</v>
+      </c>
+      <c r="D20">
+        <v>0.8038063877733501</v>
+      </c>
+      <c r="E20">
+        <v>0.6557382247212946</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="n">
+        <v>23</v>
+      </c>
+      <c r="B21">
         <v>67</v>
       </c>
-      <c r="C21" t="n">
-        <v>0.8294043729654733</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.4267165768561051</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="C21">
+        <v>0.06092309871515444</v>
+      </c>
+      <c r="D21">
+        <v>0.426716576856105</v>
+      </c>
+      <c r="E21">
+        <v>0.8294043729654725</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="n">
+        <v>24</v>
+      </c>
+      <c r="B22">
         <v>86</v>
       </c>
-      <c r="C22" t="n">
-        <v>0.7192499639843546</v>
-      </c>
-      <c r="D22" t="n">
+      <c r="C22">
+        <v>0.1706184129887596</v>
+      </c>
+      <c r="D22">
         <v>1.683853624525744</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>0.7192499639843549</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="n">
+        <v>25</v>
+      </c>
+      <c r="B23">
         <v>66</v>
       </c>
-      <c r="C23" t="n">
-        <v>0.4887190027762117</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1.140674008803199</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="C23">
+        <v>0.4899165898833819</v>
+      </c>
+      <c r="D23">
+        <v>1.140674008803198</v>
+      </c>
+      <c r="E23">
+        <v>0.4887190027762116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="n">
+        <v>26</v>
+      </c>
+      <c r="B24">
         <v>69</v>
       </c>
-      <c r="C24" t="n">
-        <v>1.715815238194145</v>
-      </c>
-      <c r="D24" t="n">
-        <v>1.602353515373593</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="C24">
+        <v>-0.4035325867946246</v>
+      </c>
+      <c r="D24">
+        <v>1.602353515373591</v>
+      </c>
+      <c r="E24">
+        <v>1.715815238194143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="n">
+        <v>27</v>
+      </c>
+      <c r="B25">
         <v>75</v>
       </c>
-      <c r="C25" t="n">
-        <v>1.264219810813608</v>
-      </c>
-      <c r="D25" t="n">
-        <v>2.485333829057352</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="C25">
+        <v>-0.1822617269622997</v>
+      </c>
+      <c r="D25">
+        <v>2.485333829057348</v>
+      </c>
+      <c r="E25">
+        <v>1.264219810813607</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="n">
+        <v>28</v>
+      </c>
+      <c r="B26">
         <v>72</v>
       </c>
-      <c r="C26" t="n">
-        <v>0.9808549446337536</v>
-      </c>
-      <c r="D26" t="n">
+      <c r="C26">
+        <v>0.04866035922866427</v>
+      </c>
+      <c r="D26">
         <v>1.930322094548117</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>0.9808549446337534</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" t="n">
+        <v>29</v>
+      </c>
+      <c r="B27">
         <v>75</v>
       </c>
-      <c r="C27" t="n">
-        <v>0.3866366398948997</v>
-      </c>
-      <c r="D27" t="n">
-        <v>1.413531659103394</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="C27">
+        <v>-0.1449050817916939</v>
+      </c>
+      <c r="D27">
+        <v>1.413531659103395</v>
+      </c>
+      <c r="E27">
+        <v>0.3866366398948996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="n">
+        <v>30</v>
+      </c>
+      <c r="B28">
         <v>71</v>
       </c>
-      <c r="C28" t="n">
-        <v>0.4914602873909301</v>
-      </c>
-      <c r="D28" t="n">
-        <v>1.62819300270981</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="C28">
+        <v>-0.07372063342003791</v>
+      </c>
+      <c r="D28">
+        <v>1.628193002709809</v>
+      </c>
+      <c r="E28">
+        <v>0.4914602873909288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="n">
+        <v>31</v>
+      </c>
+      <c r="B29">
         <v>61</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
+        <v>0.02408680631842355</v>
+      </c>
+      <c r="D29">
+        <v>0.5148854143711533</v>
+      </c>
+      <c r="E29">
         <v>0.8003563227094359</v>
       </c>
-      <c r="D29" t="n">
-        <v>0.5148854143711534</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" t="n">
+        <v>32</v>
+      </c>
+      <c r="B30">
         <v>69</v>
       </c>
-      <c r="C30" t="n">
-        <v>0.7361494804832518</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0.9022628061606567</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="C30">
+        <v>-0.6337580664246045</v>
+      </c>
+      <c r="D30">
+        <v>0.9022628061606554</v>
+      </c>
+      <c r="E30">
+        <v>0.7361494804832538</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="n">
+        <v>33</v>
+      </c>
+      <c r="B31">
         <v>70</v>
       </c>
-      <c r="C31" t="n">
-        <v>0.7587805559099208</v>
-      </c>
-      <c r="D31" t="n">
-        <v>1.629361355435436</v>
+      <c r="C31">
+        <v>0.2061585327857367</v>
+      </c>
+      <c r="D31">
+        <v>1.629361355435437</v>
+      </c>
+      <c r="E31">
+        <v>0.7587805559099209</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>